<commit_message>
Execicios do dia 20/05/2021
</commit_message>
<xml_diff>
--- a/fia/20210527/dados/Distribuicoes .xlsx
+++ b/fia/20210527/dados/Distribuicoes .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\github.com\datascience\fia\20210527\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F9B915-C3A0-49FC-A10A-5ABEAB644C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9E07C9-D31B-4862-9497-AF4C58A9E819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-465" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,9 +90,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="182" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -332,12 +331,6 @@
     <xf numFmtId="3" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -353,7 +346,13 @@
     <xf numFmtId="164" fontId="8" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1036,7 +1035,7 @@
   <dimension ref="B2:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1059,14 +1058,14 @@
     </row>
     <row r="3" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:8" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="F4" s="21" t="s">
+      <c r="C4" s="29"/>
+      <c r="F4" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="22"/>
+      <c r="G4" s="29"/>
     </row>
     <row r="5" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:8" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1074,15 +1073,15 @@
         <v>3</v>
       </c>
       <c r="C6" s="13">
-        <v>103</v>
-      </c>
-      <c r="F6" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="21" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1091,20 +1090,19 @@
         <v>5</v>
       </c>
       <c r="C7" s="14">
-        <f>99/100</f>
-        <v>0.99</v>
-      </c>
-      <c r="F7" s="24" t="str">
+        <v>0.85</v>
+      </c>
+      <c r="F7" s="22" t="str">
         <f>CONCATENATE("P(X = ",C8,")")</f>
-        <v>P(X = 100)</v>
-      </c>
-      <c r="G7" s="27">
+        <v>P(X = 10)</v>
+      </c>
+      <c r="G7" s="25">
         <f>_xlfn.BINOM.DIST(C8,C6,C7,FALSE)</f>
-        <v>6.473318558651199E-2</v>
+        <v>4.4895300689109796E-2</v>
       </c>
       <c r="H7" s="30">
         <f>G7</f>
-        <v>6.473318558651199E-2</v>
+        <v>4.4895300689109796E-2</v>
       </c>
     </row>
     <row r="8" spans="2:8" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1112,61 +1110,61 @@
         <v>4</v>
       </c>
       <c r="C8" s="15">
-        <v>100</v>
-      </c>
-      <c r="F8" s="25" t="str">
+        <v>10</v>
+      </c>
+      <c r="F8" s="23" t="str">
         <f>CONCATENATE("P(X ≤ ",C8,")")</f>
-        <v>P(X ≤ 100)</v>
-      </c>
-      <c r="G8" s="28">
+        <v>P(X ≤ 10)</v>
+      </c>
+      <c r="G8" s="26">
         <f>_xlfn.BINOM.DIST(C8,C6,C7,TRUE)</f>
-        <v>8.4974417700458646E-2</v>
+        <v>6.1705386737059831E-2</v>
       </c>
       <c r="H8" s="30">
         <f t="shared" ref="H8:H11" si="0">G8</f>
-        <v>8.4974417700458646E-2</v>
+        <v>6.1705386737059831E-2</v>
       </c>
     </row>
     <row r="9" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F9" s="25" t="str">
+      <c r="F9" s="23" t="str">
         <f>CONCATENATE("P(X &gt; ",C8,")")</f>
-        <v>P(X &gt; 100)</v>
-      </c>
-      <c r="G9" s="28">
+        <v>P(X &gt; 10)</v>
+      </c>
+      <c r="G9" s="26">
         <f>1-G8</f>
-        <v>0.91502558229954134</v>
+        <v>0.93829461326294017</v>
       </c>
       <c r="H9" s="30">
         <f t="shared" si="0"/>
-        <v>0.91502558229954134</v>
+        <v>0.93829461326294017</v>
       </c>
     </row>
     <row r="10" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F10" s="25" t="str">
+      <c r="F10" s="23" t="str">
         <f>CONCATENATE("P(X &gt;= ",C8,")")</f>
-        <v>P(X &gt;= 100)</v>
-      </c>
-      <c r="G10" s="28">
+        <v>P(X &gt;= 10)</v>
+      </c>
+      <c r="G10" s="26">
         <f>G7+G9</f>
-        <v>0.97975876788605332</v>
+        <v>0.98318991395204991</v>
       </c>
       <c r="H10" s="30">
         <f t="shared" si="0"/>
-        <v>0.97975876788605332</v>
+        <v>0.98318991395204991</v>
       </c>
     </row>
     <row r="11" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F11" s="26" t="str">
+      <c r="F11" s="24" t="str">
         <f>CONCATENATE("P(X &lt; ",C8,")")</f>
-        <v>P(X &lt; 100)</v>
-      </c>
-      <c r="G11" s="29">
+        <v>P(X &lt; 10)</v>
+      </c>
+      <c r="G11" s="27">
         <f>G8-G7</f>
-        <v>2.0241232113946656E-2</v>
+        <v>1.6810086047950035E-2</v>
       </c>
       <c r="H11" s="30">
         <f t="shared" si="0"/>
-        <v>2.0241232113946656E-2</v>
+        <v>1.6810086047950035E-2</v>
       </c>
     </row>
     <row r="12" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1225,14 +1223,14 @@
     </row>
     <row r="3" spans="2:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:7" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="F4" s="21" t="s">
+      <c r="C4" s="29"/>
+      <c r="F4" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="22"/>
+      <c r="G4" s="29"/>
     </row>
     <row r="5" spans="2:7" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:7" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1373,14 +1371,14 @@
     </row>
     <row r="3" spans="2:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:7" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="F4" s="21" t="s">
+      <c r="C4" s="29"/>
+      <c r="F4" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="22"/>
+      <c r="G4" s="29"/>
     </row>
     <row r="5" spans="2:7" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:7" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>